<commit_message>
Processing of results from on-board measurements and processing
</commit_message>
<xml_diff>
--- a/uartFFTadc/SupportFilesADC/Experiment1/Statistics.xlsx
+++ b/uartFFTadc/SupportFilesADC/Experiment1/Statistics.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tim\Documents\GitHub\MScProject_EmbeddedSystems_ConditionMonitoring\uartFFTadc\SupportFilesADC\Experiment1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\filestore.soton.ac.uk\users\tjg1g14\mydocuments\MScProject_EmbeddedSystems_ConditionMonitoring\uartFFTadc\SupportFilesADC\Experiment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8604"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8610"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -370,16 +370,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.05078125" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -390,13 +390,13 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -413,7 +413,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -430,7 +430,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -447,7 +447,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -464,7 +464,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -481,7 +481,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -498,7 +498,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -515,7 +515,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>4</v>
       </c>
@@ -532,7 +532,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>4</v>
       </c>
@@ -549,7 +549,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>4</v>
       </c>
@@ -566,7 +566,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>4</v>
       </c>
@@ -583,7 +583,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>4</v>
       </c>
@@ -600,7 +600,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>4</v>
       </c>
@@ -617,7 +617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>4</v>
       </c>
@@ -634,7 +634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>4</v>
       </c>
@@ -651,7 +651,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>4</v>
       </c>
@@ -668,7 +668,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>4</v>
       </c>
@@ -685,7 +685,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>4</v>
       </c>
@@ -702,7 +702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>4</v>
       </c>
@@ -719,7 +719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>4</v>
       </c>
@@ -736,7 +736,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>4</v>
       </c>
@@ -753,7 +753,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>4</v>
       </c>
@@ -770,7 +770,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>4</v>
       </c>
@@ -787,7 +787,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>4</v>
       </c>
@@ -804,7 +804,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>4</v>
       </c>
@@ -821,7 +821,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>4</v>
       </c>
@@ -838,7 +838,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>4</v>
       </c>
@@ -855,7 +855,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>4</v>
       </c>
@@ -872,7 +872,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>4</v>
       </c>
@@ -889,7 +889,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>4</v>
       </c>
@@ -906,7 +906,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>8</v>
       </c>
@@ -917,13 +917,13 @@
         <v>53</v>
       </c>
       <c r="E33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>8</v>
       </c>
@@ -934,13 +934,13 @@
         <v>56</v>
       </c>
       <c r="E34">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F34">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>8</v>
       </c>
@@ -951,13 +951,13 @@
         <v>57</v>
       </c>
       <c r="E35">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F35">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>8</v>
       </c>
@@ -968,13 +968,13 @@
         <v>56</v>
       </c>
       <c r="E36">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>8</v>
       </c>
@@ -985,13 +985,13 @@
         <v>56</v>
       </c>
       <c r="E37">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F37">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>8</v>
       </c>
@@ -1002,13 +1002,13 @@
         <v>55</v>
       </c>
       <c r="E38">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F38">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>8</v>
       </c>
@@ -1019,13 +1019,13 @@
         <v>54</v>
       </c>
       <c r="E39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F39">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>8</v>
       </c>
@@ -1036,13 +1036,13 @@
         <v>54</v>
       </c>
       <c r="E40">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>8</v>
       </c>
@@ -1053,13 +1053,13 @@
         <v>55</v>
       </c>
       <c r="E41">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>8</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>8</v>
       </c>
@@ -1087,13 +1087,13 @@
         <v>28</v>
       </c>
       <c r="E43">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F43">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>8</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>8</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>8</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>8</v>
       </c>
@@ -1155,13 +1155,13 @@
         <v>21</v>
       </c>
       <c r="E47">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F47">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>8</v>
       </c>
@@ -1172,13 +1172,13 @@
         <v>23</v>
       </c>
       <c r="E48">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F48">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>8</v>
       </c>
@@ -1189,13 +1189,13 @@
         <v>25</v>
       </c>
       <c r="E49">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>8</v>
       </c>
@@ -1206,13 +1206,13 @@
         <v>29</v>
       </c>
       <c r="E50">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F50">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>8</v>
       </c>
@@ -1223,13 +1223,13 @@
         <v>36</v>
       </c>
       <c r="E51">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F51">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>8</v>
       </c>
@@ -1240,10 +1240,10 @@
         <v>25</v>
       </c>
       <c r="E52">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F52">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>